<commit_message>
Changed data to from Plants to States
</commit_message>
<xml_diff>
--- a/GannEBGN632Data.xlsx
+++ b/GannEBGN632Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96829d6a2ba10c23/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zgann Git Hub\Nuclear-Power-Plant-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="747" documentId="8_{2F4914C2-AE3F-451B-BD8E-DD36BAACE476}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{5AAB17EA-BAF4-43A4-9A20-8D9DCB36874B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192EBD41-DA5C-47F4-8613-F527E23BC491}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{F37E8780-A215-4D39-A6E8-61EF379911E8}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="6" xr2:uid="{F37E8780-A215-4D39-A6E8-61EF379911E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet5!$A$1:$N$62</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="180">
   <si>
     <t>Country</t>
   </si>
@@ -3619,7 +3621,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B62"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4701,7 +4703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C944EF-F08C-4018-9264-D162291EF763}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
@@ -6887,4 +6889,1370 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464FD658-2AD9-4B1F-A7F1-FAF99AC6DEAF}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>9874.31</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>6610.86</v>
+      </c>
+      <c r="E2">
+        <v>8486.61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2">
+        <v>5894.64</v>
+      </c>
+      <c r="H2">
+        <v>5664.89</v>
+      </c>
+      <c r="I2">
+        <v>8461.02</v>
+      </c>
+      <c r="J2">
+        <v>6958.85</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>9549.65</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>6575.25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3">
+        <v>8206.67</v>
+      </c>
+      <c r="G3">
+        <v>6151.73</v>
+      </c>
+      <c r="H3">
+        <v>5512.81</v>
+      </c>
+      <c r="I3">
+        <v>8804.5</v>
+      </c>
+      <c r="J3">
+        <v>6941.48</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>8454.3700000000008</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>6794</v>
+      </c>
+      <c r="E4">
+        <v>9843.9500000000007</v>
+      </c>
+      <c r="F4">
+        <v>9293.0400000000009</v>
+      </c>
+      <c r="G4">
+        <v>7152.32</v>
+      </c>
+      <c r="H4">
+        <v>5406.69</v>
+      </c>
+      <c r="I4">
+        <v>9882.25</v>
+      </c>
+      <c r="J4">
+        <v>7198.05</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>8097.64</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>6632.6</v>
+      </c>
+      <c r="E5">
+        <v>10098.16</v>
+      </c>
+      <c r="F5">
+        <v>9675.4599999999991</v>
+      </c>
+      <c r="G5">
+        <v>7378.76</v>
+      </c>
+      <c r="H5">
+        <v>5157.91</v>
+      </c>
+      <c r="I5">
+        <v>10274.950000000001</v>
+      </c>
+      <c r="J5">
+        <v>7043.06</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <v>10480.379999999999</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>5777.68</v>
+      </c>
+      <c r="E6">
+        <v>7680.9</v>
+      </c>
+      <c r="F6">
+        <v>7271.33</v>
+      </c>
+      <c r="G6">
+        <v>5008.9399999999996</v>
+      </c>
+      <c r="H6">
+        <v>5071.5</v>
+      </c>
+      <c r="I6">
+        <v>7883.61</v>
+      </c>
+      <c r="J6">
+        <v>6097.54</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7">
+        <v>10191.23</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>6855.51</v>
+      </c>
+      <c r="E7">
+        <v>8183.5</v>
+      </c>
+      <c r="F7">
+        <v>7457.59</v>
+      </c>
+      <c r="G7">
+        <v>5701.18</v>
+      </c>
+      <c r="H7">
+        <v>6049.46</v>
+      </c>
+      <c r="I7">
+        <v>8040.17</v>
+      </c>
+      <c r="J7">
+        <v>7176.35</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>10175.790000000001</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>6643.55</v>
+      </c>
+      <c r="E8">
+        <v>8199.5</v>
+      </c>
+      <c r="F8">
+        <v>7542.58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H8">
+        <v>5813.7</v>
+      </c>
+      <c r="I8">
+        <v>8135.44</v>
+      </c>
+      <c r="J8">
+        <v>6971.7</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>9466.31</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>6138.2</v>
+      </c>
+      <c r="E9">
+        <v>8724.56</v>
+      </c>
+      <c r="F9">
+        <v>8311.86</v>
+      </c>
+      <c r="G9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H9">
+        <v>5046.4799999999996</v>
+      </c>
+      <c r="I9">
+        <v>8922.33</v>
+      </c>
+      <c r="J9">
+        <v>6512.41</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>9684.94</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>6206.14</v>
+      </c>
+      <c r="E10">
+        <v>8558.73</v>
+      </c>
+      <c r="F10">
+        <v>8095.96</v>
+      </c>
+      <c r="G10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10">
+        <v>5187.67</v>
+      </c>
+      <c r="I10">
+        <v>8704.64</v>
+      </c>
+      <c r="J10">
+        <v>6569.59</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11">
+        <v>9206.76</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>6445.12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11">
+        <v>8569.11</v>
+      </c>
+      <c r="G11">
+        <v>6381.6</v>
+      </c>
+      <c r="H11">
+        <v>5267.91</v>
+      </c>
+      <c r="I11">
+        <v>9172.94</v>
+      </c>
+      <c r="J11">
+        <v>6828.06</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12">
+        <v>9569</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>6857.51</v>
+      </c>
+      <c r="E12">
+        <v>8805.9599999999991</v>
+      </c>
+      <c r="F12">
+        <v>8126.21</v>
+      </c>
+      <c r="G12">
+        <v>6235.52</v>
+      </c>
+      <c r="H12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12">
+        <v>8710.34</v>
+      </c>
+      <c r="J12">
+        <v>7218.21</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>10487.49</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>5716.38</v>
+      </c>
+      <c r="E13">
+        <v>7644.21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13">
+        <v>4966.17</v>
+      </c>
+      <c r="H13">
+        <v>5018.53</v>
+      </c>
+      <c r="I13">
+        <v>7864.94</v>
+      </c>
+      <c r="J13">
+        <v>6035.8</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>10337.32</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>6006.73</v>
+      </c>
+      <c r="E14">
+        <v>7906.05</v>
+      </c>
+      <c r="F14">
+        <v>7439.89</v>
+      </c>
+      <c r="G14">
+        <v>5251.86</v>
+      </c>
+      <c r="H14">
+        <v>5231.3</v>
+      </c>
+      <c r="I14">
+        <v>8050.36</v>
+      </c>
+      <c r="J14">
+        <v>6334.76</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <v>9867.93</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>5896.76</v>
+      </c>
+      <c r="E15">
+        <v>8271.85</v>
+      </c>
+      <c r="F15">
+        <v>7893.03</v>
+      </c>
+      <c r="G15">
+        <v>5574.31</v>
+      </c>
+      <c r="H15">
+        <v>4952.3100000000004</v>
+      </c>
+      <c r="I15">
+        <v>8505.24</v>
+      </c>
+      <c r="J15">
+        <v>6252.72</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>9356.31</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>5881.1</v>
+      </c>
+      <c r="E16">
+        <v>8699.11</v>
+      </c>
+      <c r="F16">
+        <v>8393.4699999999993</v>
+      </c>
+      <c r="G16">
+        <v>5981.83</v>
+      </c>
+      <c r="H16">
+        <v>4760.67</v>
+      </c>
+      <c r="I16">
+        <v>9005.93</v>
+      </c>
+      <c r="J16">
+        <v>6261.08</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>9530.17</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>6339.53</v>
+      </c>
+      <c r="E17">
+        <v>8741.43</v>
+      </c>
+      <c r="F17">
+        <v>8248.76</v>
+      </c>
+      <c r="G17">
+        <v>6068.93</v>
+      </c>
+      <c r="H17">
+        <v>5267.4</v>
+      </c>
+      <c r="I17">
+        <v>8854.7199999999993</v>
+      </c>
+      <c r="J17">
+        <v>6709.32</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18">
+        <v>9706.59</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>6681.02</v>
+      </c>
+      <c r="E18">
+        <v>8655.9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G18">
+        <v>6060.11</v>
+      </c>
+      <c r="H18">
+        <v>5677.1</v>
+      </c>
+      <c r="I18">
+        <v>8618.36</v>
+      </c>
+      <c r="J18">
+        <v>7037.36</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>10296.290000000001</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>6296.08</v>
+      </c>
+      <c r="E19">
+        <v>8032.58</v>
+      </c>
+      <c r="F19">
+        <v>7477.7</v>
+      </c>
+      <c r="G19">
+        <v>5422.3</v>
+      </c>
+      <c r="H19">
+        <v>5500.44</v>
+      </c>
+      <c r="I19">
+        <v>8082.41</v>
+      </c>
+      <c r="J19">
+        <v>6623.33</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>9146</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>6219.66</v>
+      </c>
+      <c r="E20">
+        <v>9034.68</v>
+      </c>
+      <c r="F20">
+        <v>8633.66</v>
+      </c>
+      <c r="G20">
+        <v>6327.52</v>
+      </c>
+      <c r="H20">
+        <v>5023.7299999999996</v>
+      </c>
+      <c r="I20">
+        <v>9243.57</v>
+      </c>
+      <c r="J20">
+        <v>6606.39</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21">
+        <v>10464.23</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>5639.9</v>
+      </c>
+      <c r="E21">
+        <v>7624.15</v>
+      </c>
+      <c r="F21">
+        <v>7257.92</v>
+      </c>
+      <c r="G21">
+        <v>4937.33</v>
+      </c>
+      <c r="H21">
+        <v>4940.8100000000004</v>
+      </c>
+      <c r="I21">
+        <v>7870.35</v>
+      </c>
+      <c r="J21">
+        <v>5960.73</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22">
+        <v>10448.6</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>5914.06</v>
+      </c>
+      <c r="E22">
+        <v>7770.24</v>
+      </c>
+      <c r="F22">
+        <v>7321.93</v>
+      </c>
+      <c r="G22">
+        <v>5112.4799999999996</v>
+      </c>
+      <c r="H22">
+        <v>5185.88</v>
+      </c>
+      <c r="I22">
+        <v>7933.29</v>
+      </c>
+      <c r="J22">
+        <v>6235.54</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>10449.84</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>5865.33</v>
+      </c>
+      <c r="E23">
+        <v>7748.27</v>
+      </c>
+      <c r="F23">
+        <v>7314.94</v>
+      </c>
+      <c r="G23">
+        <v>5084.3900000000003</v>
+      </c>
+      <c r="H23">
+        <v>5140.6499999999996</v>
+      </c>
+      <c r="I23">
+        <v>7926.73</v>
+      </c>
+      <c r="J23">
+        <v>6186.95</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>10031.530000000001</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>6080.39</v>
+      </c>
+      <c r="E24">
+        <v>8205.68</v>
+      </c>
+      <c r="F24">
+        <v>7747.48</v>
+      </c>
+      <c r="G24">
+        <v>5537.33</v>
+      </c>
+      <c r="H24">
+        <v>5188.0600000000004</v>
+      </c>
+      <c r="I24">
+        <v>8357.5300000000007</v>
+      </c>
+      <c r="J24">
+        <v>6426.29</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>10263.620000000001</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>5932.53</v>
+      </c>
+      <c r="E25">
+        <v>7941.78</v>
+      </c>
+      <c r="F25">
+        <v>7506.76</v>
+      </c>
+      <c r="G25">
+        <v>5272.3</v>
+      </c>
+      <c r="H25">
+        <v>5132.51</v>
+      </c>
+      <c r="I25">
+        <v>8118.23</v>
+      </c>
+      <c r="J25">
+        <v>6265.65</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>10239.31</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>6453.36</v>
+      </c>
+      <c r="E26">
+        <v>8117.06</v>
+      </c>
+      <c r="F26">
+        <v>7516.39</v>
+      </c>
+      <c r="G26">
+        <v>5532.96</v>
+      </c>
+      <c r="H26">
+        <v>5639.11</v>
+      </c>
+      <c r="I26">
+        <v>8116.44</v>
+      </c>
+      <c r="J26">
+        <v>6781.54</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27">
+        <v>9893.5</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>6436.38</v>
+      </c>
+      <c r="E27">
+        <v>8436.9599999999991</v>
+      </c>
+      <c r="F27">
+        <v>7873.35</v>
+      </c>
+      <c r="G27" t="s">
+        <v>179</v>
+      </c>
+      <c r="H27">
+        <v>5492.28</v>
+      </c>
+      <c r="I27">
+        <v>8475.16</v>
+      </c>
+      <c r="J27">
+        <v>6786.12</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28">
+        <v>9133.02</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>6893.26</v>
+      </c>
+      <c r="E28">
+        <v>9231.35</v>
+      </c>
+      <c r="F28">
+        <v>8573.61</v>
+      </c>
+      <c r="G28">
+        <v>6617.77</v>
+      </c>
+      <c r="H28">
+        <v>5703.9</v>
+      </c>
+      <c r="I28">
+        <v>9156.27</v>
+      </c>
+      <c r="J28">
+        <v>7274.6</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29">
+        <v>10304.129999999999</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>6192.08</v>
+      </c>
+      <c r="E29">
+        <v>7997.97</v>
+      </c>
+      <c r="F29">
+        <v>7475.86</v>
+      </c>
+      <c r="G29">
+        <v>5369.55</v>
+      </c>
+      <c r="H29">
+        <v>5399.47</v>
+      </c>
+      <c r="I29">
+        <v>8083.11</v>
+      </c>
+      <c r="J29">
+        <v>6520.31</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>8144.89</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>5898.23</v>
+      </c>
+      <c r="E30">
+        <v>9652.91</v>
+      </c>
+      <c r="F30">
+        <v>9573.69</v>
+      </c>
+      <c r="G30">
+        <v>6964.9</v>
+      </c>
+      <c r="H30">
+        <v>4434.5</v>
+      </c>
+      <c r="I30">
+        <v>10182.629999999999</v>
+      </c>
+      <c r="J30">
+        <v>6309.07</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31">
+        <v>9613.3799999999992</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>5922.17</v>
+      </c>
+      <c r="E31">
+        <v>8502.48</v>
+      </c>
+      <c r="F31">
+        <v>8147.01</v>
+      </c>
+      <c r="G31">
+        <v>5795.16</v>
+      </c>
+      <c r="H31">
+        <v>4886.7700000000004</v>
+      </c>
+      <c r="I31">
+        <v>8759.32</v>
+      </c>
+      <c r="J31">
+        <v>6290.74</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A093BD60-6243-49D6-BCD2-F145303F8223}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>2569.8460787984218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>923.14168880716363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>1999.3447182494242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>1137.5494459940844</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <v>1060.2570238153792</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7">
+        <v>1813.985098701281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>2062.3162054383824</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>305.41171286644743</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>5879.4039982374607</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11">
+        <v>622.09735327801491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12">
+        <v>1083.1603631074922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>343.90557358356875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>867.27988565566841</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <v>2092.1768783957273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>841.48188929115963</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>604.32314318435726</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18">
+        <v>711.47623832040722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>2598.8942164371992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>391.03262206046651</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21">
+        <v>634.33616651393334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22">
+        <v>2086.1336469638836</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>2737.5838386251389</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>1083.7189811390072</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>4975.2553225018055</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>3339.6217262260252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27">
+        <v>2296.7834283024308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28">
+        <v>2518.8594875583294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29">
+        <v>1811.9537604048628</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>597.7212937209988</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31">
+        <v>605.94821382149178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>